<commit_message>
Chanegs in Driver and XLReader Class
</commit_message>
<xml_diff>
--- a/TestCases/TestCases.xlsx
+++ b/TestCases/TestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RunManager" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>Browser</t>
   </si>
@@ -35,9 +35,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>TC_Login</t>
-  </si>
-  <si>
     <t>Chrome</t>
   </si>
   <si>
@@ -87,6 +84,12 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>TC_Login1</t>
+  </si>
+  <si>
+    <t>TC_Login2</t>
   </si>
 </sst>
 </file>
@@ -430,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +446,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -460,33 +463,33 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3"/>
     </row>
@@ -497,15 +500,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -513,34 +516,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
+      <c r="A1" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
-        <v>13</v>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -563,16 +571,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>